<commit_message>
Agregúe los datos más recientes
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1546</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1567</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10823" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10970" uniqueCount="390">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1172,6 +1172,18 @@
   <si>
     <t xml:space="preserve">Luis Ángel Malagón    </t>
   </si>
+  <si>
+    <t>José Raúl Zúñiga</t>
+  </si>
+  <si>
+    <t>Luis Ángel Malagón</t>
+  </si>
+  <si>
+    <t>Alexis Gutiérrez</t>
+  </si>
+  <si>
+    <t>Brian Rodríguez</t>
+  </si>
 </sst>
 </file>
 
@@ -1348,10 +1360,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1359,13 +1371,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1373,13 +1385,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1524,8 +1536,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1546" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1546"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1567" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1567"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -41928,38 +41940,584 @@
       </c>
     </row>
     <row r="1546">
-      <c r="A1546" s="19">
+      <c r="A1546" s="15">
         <v>45877.38914206019</v>
       </c>
-      <c r="B1546" s="20" t="s">
+      <c r="B1546" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C1546" s="20" t="s">
+      <c r="C1546" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="D1546" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1546" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1546" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1546" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1546" s="21" t="s">
+      <c r="D1546" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1546" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1546" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1546" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1546" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" s="12">
+        <v>45880.351948807875</v>
+      </c>
+      <c r="B1547" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1547" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1547" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1547" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1547" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1547" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1547" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" s="15">
+        <v>45880.35497219907</v>
+      </c>
+      <c r="B1548" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1548" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1548" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1548" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1548" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1548" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1548" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" s="12">
+        <v>45880.35605615741</v>
+      </c>
+      <c r="B1549" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1549" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1549" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1549" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1549" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1549" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1549" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" s="15">
+        <v>45880.3568934375</v>
+      </c>
+      <c r="B1550" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1550" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1550" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1550" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1550" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1550" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1550" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" s="12">
+        <v>45880.36914304398</v>
+      </c>
+      <c r="B1551" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1551" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1551" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1551" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1551" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1551" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1551" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" s="15">
+        <v>45880.37883199074</v>
+      </c>
+      <c r="B1552" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1552" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1552" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1552" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1552" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1552" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1552" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1553">
+      <c r="A1553" s="12">
+        <v>45880.38362291666</v>
+      </c>
+      <c r="B1553" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1553" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1553" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1553" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1553" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1553" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1553" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" s="15">
+        <v>45880.384631030094</v>
+      </c>
+      <c r="B1554" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1554" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1554" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1554" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1554" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1554" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1554" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" s="12">
+        <v>45880.38479652778</v>
+      </c>
+      <c r="B1555" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1555" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1555" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1555" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1555" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1555" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1555" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1556">
+      <c r="A1556" s="15">
+        <v>45880.38497909722</v>
+      </c>
+      <c r="B1556" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1556" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1556" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1556" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1556" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1556" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1556" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1557">
+      <c r="A1557" s="12">
+        <v>45880.38532104167</v>
+      </c>
+      <c r="B1557" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1557" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1557" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1557" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1557" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1557" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1557" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1558">
+      <c r="A1558" s="15">
+        <v>45880.387728368056</v>
+      </c>
+      <c r="B1558" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1558" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1558" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1558" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1558" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1558" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1558" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1559">
+      <c r="A1559" s="12">
+        <v>45880.38928990741</v>
+      </c>
+      <c r="B1559" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1559" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1559" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1559" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1559" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1559" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1559" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1560">
+      <c r="A1560" s="15">
+        <v>45880.389651053236</v>
+      </c>
+      <c r="B1560" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1560" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1560" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1560" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1560" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1560" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1560" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1561">
+      <c r="A1561" s="12">
+        <v>45880.39028413194</v>
+      </c>
+      <c r="B1561" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1561" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1561" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1561" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1561" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1561" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1561" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1562">
+      <c r="A1562" s="15">
+        <v>45880.39076241898</v>
+      </c>
+      <c r="B1562" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1562" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1562" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1562" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1562" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1562" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1562" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" s="12">
+        <v>45880.39178005787</v>
+      </c>
+      <c r="B1563" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1563" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1563" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1563" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1563" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1563" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1563" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1564">
+      <c r="A1564" s="15">
+        <v>45880.39196759259</v>
+      </c>
+      <c r="B1564" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1564" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1564" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1564" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1564" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1564" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1564" s="17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1565">
+      <c r="A1565" s="12">
+        <v>45880.40407255787</v>
+      </c>
+      <c r="B1565" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1565" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1565" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1565" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1565" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1565" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1565" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" s="15">
+        <v>45880.41896456019</v>
+      </c>
+      <c r="B1566" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1566" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1566" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1566" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1566" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1566" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1566" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" s="19">
+        <v>45880.41930699074</v>
+      </c>
+      <c r="B1567" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1567" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1567" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1567" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1567" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1567" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1567" s="21" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1646">
+  <conditionalFormatting sqref="D1:D1667">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1646">
+  <conditionalFormatting sqref="G2:G1667">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added workflow using yml file.
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1567</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1584</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10970" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11089" uniqueCount="390">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1213,7 +1213,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border/>
     <border>
       <left style="thin">
@@ -1360,10 +1360,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1371,13 +1371,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1385,13 +1385,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFDD7E6B"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDD7E6B"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDD7E6B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1401,7 +1415,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1466,6 +1480,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1536,8 +1553,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1567" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1567"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1584" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1584"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -42486,38 +42503,480 @@
       </c>
     </row>
     <row r="1567">
-      <c r="A1567" s="19">
+      <c r="A1567" s="12">
         <v>45880.41930699074</v>
       </c>
-      <c r="B1567" s="20" t="s">
+      <c r="B1567" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="C1567" s="20" t="s">
+      <c r="C1567" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="D1567" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1567" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1567" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1567" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1567" s="21" t="s">
-        <v>13</v>
+      <c r="D1567" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1567" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1567" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1567" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1567" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1568">
+      <c r="A1568" s="15">
+        <v>45881.34970086806</v>
+      </c>
+      <c r="B1568" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1568" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1568" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1568" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1568" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1568" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1568" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1569">
+      <c r="A1569" s="12">
+        <v>45881.35944141204</v>
+      </c>
+      <c r="B1569" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1569" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1569" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1569" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1569" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1569" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1569" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1570">
+      <c r="A1570" s="15">
+        <v>45881.35983332176</v>
+      </c>
+      <c r="B1570" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1570" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1570" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1570" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1570" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1570" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1570" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1571">
+      <c r="A1571" s="12">
+        <v>45881.36059590278</v>
+      </c>
+      <c r="B1571" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1571" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1571" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1571" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1571" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1571" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1571" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1572">
+      <c r="A1572" s="15">
+        <v>45881.36090865741</v>
+      </c>
+      <c r="B1572" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1572" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1572" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1572" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1572" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1572" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1572" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1573">
+      <c r="A1573" s="12">
+        <v>45881.367832013886</v>
+      </c>
+      <c r="B1573" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1573" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1573" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1573" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1573" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1573" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1573" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1574">
+      <c r="A1574" s="15">
+        <v>45881.369973356486</v>
+      </c>
+      <c r="B1574" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1574" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1574" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1574" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1574" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1574" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1574" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1575">
+      <c r="A1575" s="12">
+        <v>45881.3724607176</v>
+      </c>
+      <c r="B1575" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1575" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1575" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1575" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1575" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1575" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1575" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1576">
+      <c r="A1576" s="15">
+        <v>45881.372934328705</v>
+      </c>
+      <c r="B1576" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1576" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1576" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1576" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1576" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1576" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1576" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1577">
+      <c r="A1577" s="12">
+        <v>45881.37317238426</v>
+      </c>
+      <c r="B1577" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1577" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1577" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1577" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1577" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1577" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1577" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" s="15">
+        <v>45881.373618541664</v>
+      </c>
+      <c r="B1578" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1578" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1578" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1578" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1578" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1578" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1578" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" s="12">
+        <v>45881.37730723379</v>
+      </c>
+      <c r="B1579" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1579" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1579" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1579" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1579" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1579" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1579" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1580">
+      <c r="A1580" s="15">
+        <v>45881.37750016204</v>
+      </c>
+      <c r="B1580" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1580" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1580" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1580" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1580" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1580" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1580" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" s="12">
+        <v>45881.37838711806</v>
+      </c>
+      <c r="B1581" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1581" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1581" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1581" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1581" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1581" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1581" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" s="15">
+        <v>45881.38025357639</v>
+      </c>
+      <c r="B1582" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1582" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1582" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1582" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1582" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1582" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1582" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1583">
+      <c r="A1583" s="12">
+        <v>45881.38045846065</v>
+      </c>
+      <c r="B1583" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1583" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1583" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1583" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1583" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1583" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1583" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1584">
+      <c r="A1584" s="19">
+        <v>45881.381669062495</v>
+      </c>
+      <c r="B1584" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1584" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1584" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1584" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1584" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1584" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1584" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1667">
+  <conditionalFormatting sqref="D1:D1684">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1667">
+  <conditionalFormatting sqref="G2:G1684">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Asegurándome que todo esté al día
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1584</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1591</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11089" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11138" uniqueCount="391">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1184,6 +1184,9 @@
   <si>
     <t>Brian Rodríguez</t>
   </si>
+  <si>
+    <t>Allan Saint-Maximin</t>
+  </si>
 </sst>
 </file>
 
@@ -1213,7 +1216,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -1360,10 +1363,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1371,13 +1374,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1385,27 +1388,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFDD7E6B"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFDD7E6B"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFDD7E6B"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1415,7 +1404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1480,9 +1469,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1553,8 +1539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1584" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1584"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1591" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1591"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -42945,38 +42931,220 @@
       </c>
     </row>
     <row r="1584">
-      <c r="A1584" s="19">
+      <c r="A1584" s="15">
         <v>45881.381669062495</v>
       </c>
-      <c r="B1584" s="20" t="s">
+      <c r="B1584" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C1584" s="20" t="s">
+      <c r="C1584" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="D1584" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1584" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1584" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1584" s="21" t="s">
+      <c r="D1584" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1584" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1584" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1584" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H1584" s="22" t="s">
+      <c r="H1584" s="17" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="1585">
+      <c r="A1585" s="12">
+        <v>45881.38301464121</v>
+      </c>
+      <c r="B1585" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1585" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1585" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1585" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1585" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1585" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1585" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1586">
+      <c r="A1586" s="15">
+        <v>45881.383263483796</v>
+      </c>
+      <c r="B1586" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1586" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1586" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1586" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1586" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1586" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1586" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1587">
+      <c r="A1587" s="12">
+        <v>45881.38395292824</v>
+      </c>
+      <c r="B1587" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1587" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1587" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1587" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1587" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1587" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1587" s="14" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="1588">
+      <c r="A1588" s="15">
+        <v>45881.39453532407</v>
+      </c>
+      <c r="B1588" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1588" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1588" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1588" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1588" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1588" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1588" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1589">
+      <c r="A1589" s="12">
+        <v>45881.401105613426</v>
+      </c>
+      <c r="B1589" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1589" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1589" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1589" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1589" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1589" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1589" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1590">
+      <c r="A1590" s="15">
+        <v>45881.401315358795</v>
+      </c>
+      <c r="B1590" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1590" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1590" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1590" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1590" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1590" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1590" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1591">
+      <c r="A1591" s="19">
+        <v>45881.40468253472</v>
+      </c>
+      <c r="B1591" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1591" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1591" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1591" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1591" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1591" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1591" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1684">
+  <conditionalFormatting sqref="D1:D1691">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1684">
+  <conditionalFormatting sqref="G2:G1691">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Cambié workflow y path en .py
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1591</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1611</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11138" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11278" uniqueCount="391">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1216,7 +1216,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border/>
     <border>
       <left style="thin">
@@ -1388,6 +1388,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFDD7E6B"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDD7E6B"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDD7E6B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
@@ -1404,7 +1418,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1469,6 +1483,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1539,8 +1556,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1591" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1591"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1611" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1611"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -43113,38 +43130,558 @@
       </c>
     </row>
     <row r="1591">
-      <c r="A1591" s="19">
+      <c r="A1591" s="12">
         <v>45881.40468253472</v>
       </c>
-      <c r="B1591" s="20" t="s">
+      <c r="B1591" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="C1591" s="20" t="s">
+      <c r="C1591" s="13" t="s">
         <v>390</v>
       </c>
-      <c r="D1591" s="20" t="s">
+      <c r="D1591" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E1591" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1591" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1591" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1591" s="21" t="s">
-        <v>13</v>
+      <c r="E1591" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1591" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1591" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1591" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1592">
+      <c r="A1592" s="15">
+        <v>45882.35950185185</v>
+      </c>
+      <c r="B1592" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1592" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1592" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1592" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1592" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1592" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1592" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1593">
+      <c r="A1593" s="12">
+        <v>45882.35975902778</v>
+      </c>
+      <c r="B1593" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1593" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1593" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1593" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1593" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1593" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1593" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1594">
+      <c r="A1594" s="15">
+        <v>45882.35998528935</v>
+      </c>
+      <c r="B1594" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1594" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1594" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1594" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1594" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1594" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1594" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1595">
+      <c r="A1595" s="12">
+        <v>45882.36560993055</v>
+      </c>
+      <c r="B1595" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1595" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1595" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1595" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1595" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1595" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1595" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1596">
+      <c r="A1596" s="15">
+        <v>45882.368365567134</v>
+      </c>
+      <c r="B1596" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1596" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1596" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1596" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1596" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1596" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1596" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1597">
+      <c r="A1597" s="12">
+        <v>45882.36938403935</v>
+      </c>
+      <c r="B1597" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1597" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1597" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1597" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1597" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1597" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1597" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1598">
+      <c r="A1598" s="15">
+        <v>45882.37654596065</v>
+      </c>
+      <c r="B1598" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1598" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1598" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1598" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1598" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1598" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1598" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1599">
+      <c r="A1599" s="12">
+        <v>45882.37705993056</v>
+      </c>
+      <c r="B1599" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1599" s="13" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1599" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1599" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1599" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1599" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1599" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1600">
+      <c r="A1600" s="15">
+        <v>45882.38646496528</v>
+      </c>
+      <c r="B1600" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1600" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1600" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1600" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1600" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1600" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1600" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1601">
+      <c r="A1601" s="12">
+        <v>45882.388083645834</v>
+      </c>
+      <c r="B1601" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1601" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1601" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1601" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1601" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1601" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1601" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1602">
+      <c r="A1602" s="15">
+        <v>45882.389070324076</v>
+      </c>
+      <c r="B1602" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1602" s="16" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1602" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1602" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1602" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1602" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1602" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1603">
+      <c r="A1603" s="12">
+        <v>45882.389471435185</v>
+      </c>
+      <c r="B1603" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1603" s="13" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1603" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1603" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1603" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1603" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1603" s="14" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1604">
+      <c r="A1604" s="15">
+        <v>45882.39004302083</v>
+      </c>
+      <c r="B1604" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1604" s="16" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1604" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1604" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1604" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1604" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1604" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1605">
+      <c r="A1605" s="12">
+        <v>45882.3903350926</v>
+      </c>
+      <c r="B1605" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1605" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1605" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1605" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1605" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1605" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1605" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1606">
+      <c r="A1606" s="15">
+        <v>45882.39110766204</v>
+      </c>
+      <c r="B1606" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1606" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1606" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1606" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1606" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1606" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1606" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1607">
+      <c r="A1607" s="12">
+        <v>45882.391556539354</v>
+      </c>
+      <c r="B1607" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1607" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1607" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1607" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1607" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1607" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1607" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1608">
+      <c r="A1608" s="15">
+        <v>45882.39249424769</v>
+      </c>
+      <c r="B1608" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1608" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1608" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1608" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1608" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1608" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1608" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1609">
+      <c r="A1609" s="12">
+        <v>45882.39509273148</v>
+      </c>
+      <c r="B1609" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1609" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1609" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1609" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1609" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1609" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1609" s="14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="1610">
+      <c r="A1610" s="15">
+        <v>45882.395311458335</v>
+      </c>
+      <c r="B1610" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1610" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1610" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1610" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1610" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1610" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1610" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1611">
+      <c r="A1611" s="19">
+        <v>45882.40090146991</v>
+      </c>
+      <c r="B1611" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1611" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1611" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1611" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1611" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1611" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1611" s="22" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1691">
+  <conditionalFormatting sqref="D1:D1711">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1691">
+  <conditionalFormatting sqref="G2:G1711">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
volví a cambiar workflow
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1611</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1634</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11278" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11439" uniqueCount="391">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1216,7 +1216,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -1363,10 +1363,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1374,13 +1374,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1388,27 +1388,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFDD7E6B"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFDD7E6B"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFDD7E6B"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFF8F9FA"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1418,7 +1404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1483,9 +1469,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1556,8 +1539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1611" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1611"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1634" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1634"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -43650,38 +43633,636 @@
       </c>
     </row>
     <row r="1611">
-      <c r="A1611" s="19">
+      <c r="A1611" s="12">
         <v>45882.40090146991</v>
       </c>
-      <c r="B1611" s="20" t="s">
+      <c r="B1611" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1611" s="20" t="s">
+      <c r="C1611" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="D1611" s="20" t="s">
+      <c r="D1611" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E1611" s="20" t="s">
+      <c r="E1611" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F1611" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1611" s="21" t="s">
+      <c r="F1611" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1611" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H1611" s="22" t="s">
+      <c r="H1611" s="14" t="s">
         <v>166</v>
       </c>
     </row>
+    <row r="1612">
+      <c r="A1612" s="15">
+        <v>45883.34490467593</v>
+      </c>
+      <c r="B1612" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1612" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1612" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1612" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1612" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1612" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1612" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1613">
+      <c r="A1613" s="12">
+        <v>45883.35785920139</v>
+      </c>
+      <c r="B1613" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1613" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1613" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1613" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1613" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1613" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1613" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1614">
+      <c r="A1614" s="15">
+        <v>45883.358326435184</v>
+      </c>
+      <c r="B1614" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1614" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1614" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1614" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1614" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1614" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1614" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1615">
+      <c r="A1615" s="12">
+        <v>45883.35856253472</v>
+      </c>
+      <c r="B1615" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1615" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1615" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1615" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1615" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1615" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1615" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1616">
+      <c r="A1616" s="15">
+        <v>45883.367815034726</v>
+      </c>
+      <c r="B1616" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1616" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1616" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1616" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1616" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1616" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1616" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1617">
+      <c r="A1617" s="12">
+        <v>45883.371031863426</v>
+      </c>
+      <c r="B1617" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1617" s="13" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1617" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1617" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1617" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1617" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1617" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" s="15">
+        <v>45883.37126668981</v>
+      </c>
+      <c r="B1618" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1618" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1618" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1618" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1618" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1618" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1618" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1619">
+      <c r="A1619" s="12">
+        <v>45883.371949699074</v>
+      </c>
+      <c r="B1619" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1619" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1619" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1619" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1619" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1619" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1619" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" s="15">
+        <v>45883.372554699075</v>
+      </c>
+      <c r="B1620" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1620" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1620" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1620" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1620" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1620" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1620" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" s="12">
+        <v>45883.37275708333</v>
+      </c>
+      <c r="B1621" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1621" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1621" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1621" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1621" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1621" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1621" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1622">
+      <c r="A1622" s="15">
+        <v>45883.373002824075</v>
+      </c>
+      <c r="B1622" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1622" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1622" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1622" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1622" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1622" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1622" s="17" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="1623">
+      <c r="A1623" s="12">
+        <v>45883.374393125</v>
+      </c>
+      <c r="B1623" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1623" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1623" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1623" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1623" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1623" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1623" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1624">
+      <c r="A1624" s="15">
+        <v>45883.37459864584</v>
+      </c>
+      <c r="B1624" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1624" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D1624" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1624" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1624" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1624" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1624" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" s="12">
+        <v>45883.37485944445</v>
+      </c>
+      <c r="B1625" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1625" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1625" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1625" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1625" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1625" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1625" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" s="15">
+        <v>45883.376316967595</v>
+      </c>
+      <c r="B1626" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1626" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1626" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1626" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1626" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1626" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1626" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" s="12">
+        <v>45883.38367258102</v>
+      </c>
+      <c r="B1627" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1627" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="D1627" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1627" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1627" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1627" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1627" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" s="15">
+        <v>45883.385100266205</v>
+      </c>
+      <c r="B1628" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1628" s="16" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1628" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1628" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1628" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1628" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1628" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" s="12">
+        <v>45883.391343923606</v>
+      </c>
+      <c r="B1629" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1629" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1629" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1629" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1629" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1629" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1629" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" s="15">
+        <v>45883.40386751157</v>
+      </c>
+      <c r="B1630" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1630" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1630" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1630" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1630" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1630" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1630" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" s="12">
+        <v>45883.404108622686</v>
+      </c>
+      <c r="B1631" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1631" s="13" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1631" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1631" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1631" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1631" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1631" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" s="15">
+        <v>45883.41425511574</v>
+      </c>
+      <c r="B1632" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1632" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1632" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1632" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1632" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1632" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1632" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" s="12">
+        <v>45883.41445065972</v>
+      </c>
+      <c r="B1633" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1633" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1633" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1633" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1633" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1633" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1633" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" s="19">
+        <v>45883.414607280094</v>
+      </c>
+      <c r="B1634" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1634" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="D1634" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1634" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1634" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1634" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1634" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1711">
+  <conditionalFormatting sqref="D1:D1734">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1711">
+  <conditionalFormatting sqref="G2:G1734">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Cambios al workflow para commit sheet despu'es de download
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1634</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1650</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11439" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11551" uniqueCount="391">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1216,7 +1216,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border/>
     <border>
       <left style="thin">
@@ -1388,6 +1388,20 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFDD7E6B"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFDD7E6B"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFDD7E6B"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
@@ -1404,7 +1418,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1469,6 +1483,9 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1539,8 +1556,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1634" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1634"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1650" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1650"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -44231,38 +44248,454 @@
       </c>
     </row>
     <row r="1634">
-      <c r="A1634" s="19">
+      <c r="A1634" s="15">
         <v>45883.414607280094</v>
       </c>
-      <c r="B1634" s="20" t="s">
+      <c r="B1634" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C1634" s="20" t="s">
+      <c r="C1634" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="D1634" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1634" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1634" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1634" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1634" s="21" t="s">
-        <v>13</v>
+      <c r="D1634" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1634" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1634" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1634" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1634" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" s="12">
+        <v>45884.33805715278</v>
+      </c>
+      <c r="B1635" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1635" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="D1635" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1635" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1635" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1635" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1635" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1636">
+      <c r="A1636" s="15">
+        <v>45884.341288055555</v>
+      </c>
+      <c r="B1636" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1636" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1636" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1636" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1636" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1636" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1636" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1637">
+      <c r="A1637" s="12">
+        <v>45884.34146255787</v>
+      </c>
+      <c r="B1637" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1637" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1637" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1637" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1637" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1637" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1637" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1638">
+      <c r="A1638" s="15">
+        <v>45884.341663900464</v>
+      </c>
+      <c r="B1638" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1638" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1638" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1638" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1638" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1638" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1638" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1639">
+      <c r="A1639" s="12">
+        <v>45884.341975069445</v>
+      </c>
+      <c r="B1639" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1639" s="13" t="s">
+        <v>386</v>
+      </c>
+      <c r="D1639" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1639" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1639" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1639" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1639" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1640">
+      <c r="A1640" s="15">
+        <v>45884.342484016204</v>
+      </c>
+      <c r="B1640" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1640" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1640" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1640" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1640" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1640" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1640" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1641">
+      <c r="A1641" s="12">
+        <v>45884.344802974534</v>
+      </c>
+      <c r="B1641" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1641" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1641" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1641" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1641" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1641" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1641" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1642">
+      <c r="A1642" s="15">
+        <v>45884.347059594904</v>
+      </c>
+      <c r="B1642" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1642" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1642" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1642" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1642" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1642" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1642" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1643">
+      <c r="A1643" s="12">
+        <v>45884.34791650463</v>
+      </c>
+      <c r="B1643" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1643" s="13" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1643" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1643" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1643" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1643" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1643" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1644">
+      <c r="A1644" s="15">
+        <v>45884.3486690625</v>
+      </c>
+      <c r="B1644" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1644" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1644" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1644" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1644" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1644" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1644" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1645">
+      <c r="A1645" s="12">
+        <v>45884.348960682866</v>
+      </c>
+      <c r="B1645" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1645" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="D1645" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1645" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1645" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1645" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1645" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1646">
+      <c r="A1646" s="15">
+        <v>45884.35048953704</v>
+      </c>
+      <c r="B1646" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1646" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="D1646" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1646" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1646" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1646" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1646" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1647">
+      <c r="A1647" s="12">
+        <v>45884.3509165162</v>
+      </c>
+      <c r="B1647" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1647" s="13" t="s">
+        <v>389</v>
+      </c>
+      <c r="D1647" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1647" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1647" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1647" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1647" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1648">
+      <c r="A1648" s="15">
+        <v>45884.35251921296</v>
+      </c>
+      <c r="B1648" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1648" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1648" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1648" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1648" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1648" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1648" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1649">
+      <c r="A1649" s="12">
+        <v>45884.369775196756</v>
+      </c>
+      <c r="B1649" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1649" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D1649" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1649" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1649" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1649" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1649" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1650">
+      <c r="A1650" s="19">
+        <v>45884.376228090274</v>
+      </c>
+      <c r="B1650" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1650" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1650" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1650" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1650" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1650" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1650" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1734">
+  <conditionalFormatting sqref="D1:D1750">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1734">
+  <conditionalFormatting sqref="G2:G1750">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
cambié workflow y .py file
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1650</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1653</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11551" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11572" uniqueCount="391">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1216,7 +1216,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -1363,10 +1363,10 @@
         <color rgb="FF442F65"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1374,13 +1374,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1388,27 +1388,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFDD7E6B"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFDD7E6B"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFDD7E6B"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF442F65"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="thin">
         <color rgb="FF442F65"/>
       </right>
       <top style="thin">
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFF8F9FA"/>
       </top>
       <bottom style="thin">
         <color rgb="FF442F65"/>
@@ -1418,7 +1404,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1483,9 +1469,6 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="13" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -1556,8 +1539,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1650" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1650"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1653" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1653"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -44664,38 +44647,116 @@
       </c>
     </row>
     <row r="1650">
-      <c r="A1650" s="19">
+      <c r="A1650" s="15">
         <v>45884.376228090274</v>
       </c>
-      <c r="B1650" s="20" t="s">
+      <c r="B1650" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C1650" s="20" t="s">
+      <c r="C1650" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="D1650" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1650" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1650" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1650" s="21" t="s">
+      <c r="D1650" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1650" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1650" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1650" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H1650" s="22" t="s">
+      <c r="H1650" s="17" t="s">
         <v>60</v>
       </c>
     </row>
+    <row r="1651">
+      <c r="A1651" s="12">
+        <v>45884.41920474537</v>
+      </c>
+      <c r="B1651" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1651" s="13" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1651" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1651" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1651" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1651" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1651" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1652">
+      <c r="A1652" s="15">
+        <v>45887.37138094907</v>
+      </c>
+      <c r="B1652" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1652" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="D1652" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1652" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1652" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1652" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1652" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="1653">
+      <c r="A1653" s="19">
+        <v>45887.3809612037</v>
+      </c>
+      <c r="B1653" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1653" s="20" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1653" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1653" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1653" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1653" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1653" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1750">
+  <conditionalFormatting sqref="D1:D1753">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1750">
+  <conditionalFormatting sqref="G2:G1753">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Resolve binary conflict on XLSX: keep local (stashed) version
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1781</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$1775</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12468" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12426" uniqueCount="392">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1542,8 +1542,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1781" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$1781"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H1775" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$1775"/>
   <tableColumns count="8">
     <tableColumn name="Marca temporal" id="1"/>
     <tableColumn name="Día de la Semana" id="2"/>
@@ -47900,194 +47900,38 @@
       </c>
     </row>
     <row r="1775">
-      <c r="A1775" s="12">
+      <c r="A1775" s="19">
         <v>45895.381882974536</v>
       </c>
-      <c r="B1775" s="13" t="s">
+      <c r="B1775" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C1775" s="13" t="s">
+      <c r="C1775" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="D1775" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1775" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1775" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1775" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1775" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1776">
-      <c r="A1776" s="15">
-        <v>45895.38637034722</v>
-      </c>
-      <c r="B1776" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1776" s="16" t="s">
-        <v>216</v>
-      </c>
-      <c r="D1776" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1776" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1776" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1776" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1776" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1777">
-      <c r="A1777" s="12">
-        <v>45895.38965509259</v>
-      </c>
-      <c r="B1777" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1777" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="D1777" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1777" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1777" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1777" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1777" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1778">
-      <c r="A1778" s="15">
-        <v>45895.396348888884</v>
-      </c>
-      <c r="B1778" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1778" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="D1778" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1778" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1778" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1778" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1778" s="17" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="1779">
-      <c r="A1779" s="12">
-        <v>45895.397699016205</v>
-      </c>
-      <c r="B1779" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1779" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="D1779" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1779" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1779" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1779" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1779" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1780">
-      <c r="A1780" s="15">
-        <v>45895.40102993055</v>
-      </c>
-      <c r="B1780" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1780" s="16" t="s">
-        <v>387</v>
-      </c>
-      <c r="D1780" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1780" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1780" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1780" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1780" s="17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="1781">
-      <c r="A1781" s="19">
-        <v>45895.402354074075</v>
-      </c>
-      <c r="B1781" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C1781" s="20" t="s">
-        <v>171</v>
-      </c>
-      <c r="D1781" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1781" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1781" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1781" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1781" s="21" t="s">
+      <c r="D1775" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1775" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1775" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1775" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1775" s="21" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1881">
+  <conditionalFormatting sqref="D1:D1875">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G1881">
+  <conditionalFormatting sqref="G2:G1875">
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>

<commit_message>
actualicé workflow y .py
</commit_message>
<xml_diff>
--- a/data/bienestar_jugador_primer_equipo_respuestas.xlsx
+++ b/data/bienestar_jugador_primer_equipo_respuestas.xlsx
@@ -6,14 +6,14 @@
     <sheet state="visible" name="Respuestas de formulario 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$2662</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Respuestas de formulario 1'!$A$1:$H$2709</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18635" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18964" uniqueCount="396">
   <si>
     <t>Marca temporal</t>
   </si>
@@ -1344,8 +1344,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H2662" displayName="Form_Responses1" name="Form_Responses1" id="1">
-  <autoFilter ref="$A$1:$H$2662">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:H2709" displayName="Form_Responses1" name="Form_Responses1" id="1">
+  <autoFilter ref="$A$1:$H$2709">
     <filterColumn colId="2">
       <filters>
         <filter val="Álvaro fidalgo"/>
@@ -42932,7 +42932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1591" ht="22.5" customHeight="1">
+    <row r="1591" ht="22.5" hidden="1" customHeight="1">
       <c r="A1591" s="5">
         <v>45881.40468253472</v>
       </c>
@@ -43270,7 +43270,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="1604" ht="22.5" customHeight="1">
+    <row r="1604" ht="22.5" hidden="1" customHeight="1">
       <c r="A1604" s="5">
         <v>45882.39004302083</v>
       </c>
@@ -43764,7 +43764,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="1623" ht="22.5" customHeight="1">
+    <row r="1623" ht="22.5" hidden="1" customHeight="1">
       <c r="A1623" s="5">
         <v>45883.374393125</v>
       </c>
@@ -44492,7 +44492,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="1651" ht="22.5" customHeight="1">
+    <row r="1651" ht="22.5" hidden="1" customHeight="1">
       <c r="A1651" s="5">
         <v>45884.41920474537</v>
       </c>
@@ -44544,7 +44544,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="1653" ht="22.5" customHeight="1">
+    <row r="1653" ht="22.5" hidden="1" customHeight="1">
       <c r="A1653" s="5">
         <v>45887.3809612037</v>
       </c>
@@ -44986,7 +44986,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1670" ht="22.5" customHeight="1">
+    <row r="1670" ht="22.5" hidden="1" customHeight="1">
       <c r="A1670" s="5">
         <v>45888.39140821759</v>
       </c>
@@ -45610,7 +45610,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="1694" ht="22.5" customHeight="1">
+    <row r="1694" ht="22.5" hidden="1" customHeight="1">
       <c r="A1694" s="5">
         <v>45889.379339872685</v>
       </c>
@@ -46234,7 +46234,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1718" ht="22.5" customHeight="1">
+    <row r="1718" ht="22.5" hidden="1" customHeight="1">
       <c r="A1718" s="5">
         <v>45890.392384004634</v>
       </c>
@@ -46858,7 +46858,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1742" ht="22.5" customHeight="1">
+    <row r="1742" ht="22.5" hidden="1" customHeight="1">
       <c r="A1742" s="5">
         <v>45891.3899556713</v>
       </c>
@@ -47404,7 +47404,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1763" ht="22.5" customHeight="1">
+    <row r="1763" ht="22.5" hidden="1" customHeight="1">
       <c r="A1763" s="5">
         <v>45892.36715967592</v>
       </c>
@@ -47768,7 +47768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1777" ht="22.5" customHeight="1">
+    <row r="1777" ht="22.5" hidden="1" customHeight="1">
       <c r="A1777" s="5">
         <v>45895.38965509259</v>
       </c>
@@ -48080,7 +48080,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1789" ht="22.5" customHeight="1">
+    <row r="1789" ht="22.5" hidden="1" customHeight="1">
       <c r="A1789" s="5">
         <v>45896.371080972225</v>
       </c>
@@ -48704,7 +48704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1813" ht="22.5" customHeight="1">
+    <row r="1813" ht="22.5" hidden="1" customHeight="1">
       <c r="A1813" s="5">
         <v>45897.380201249995</v>
       </c>
@@ -49328,7 +49328,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1837" ht="22.5" customHeight="1">
+    <row r="1837" ht="22.5" hidden="1" customHeight="1">
       <c r="A1837" s="5">
         <v>45898.389731979165</v>
       </c>
@@ -49744,7 +49744,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1853" ht="22.5" customHeight="1">
+    <row r="1853" ht="22.5" hidden="1" customHeight="1">
       <c r="A1853" s="5">
         <v>45904.40915924768</v>
       </c>
@@ -49900,7 +49900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1859" ht="22.5" customHeight="1">
+    <row r="1859" ht="22.5" hidden="1" customHeight="1">
       <c r="A1859" s="5">
         <v>45908.398801041665</v>
       </c>
@@ -50446,7 +50446,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1880" ht="22.5" customHeight="1">
+    <row r="1880" ht="22.5" hidden="1" customHeight="1">
       <c r="A1880" s="5">
         <v>45909.38609510417</v>
       </c>
@@ -50836,7 +50836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1895" ht="22.5" customHeight="1">
+    <row r="1895" ht="22.5" hidden="1" customHeight="1">
       <c r="A1895" s="5">
         <v>45910.38872837963</v>
       </c>
@@ -51746,7 +51746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1930" ht="22.5" customHeight="1">
+    <row r="1930" ht="22.5" hidden="1" customHeight="1">
       <c r="A1930" s="5">
         <v>45911.399243576394</v>
       </c>
@@ -52188,7 +52188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1947" ht="22.5" customHeight="1">
+    <row r="1947" ht="22.5" hidden="1" customHeight="1">
       <c r="A1947" s="5">
         <v>45912.37963631944</v>
       </c>
@@ -52838,7 +52838,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="1972" ht="22.5" customHeight="1">
+    <row r="1972" ht="22.5" hidden="1" customHeight="1">
       <c r="A1972" s="5">
         <v>45915.40587287037</v>
       </c>
@@ -53098,7 +53098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="1982" ht="22.5" customHeight="1">
+    <row r="1982" ht="22.5" hidden="1" customHeight="1">
       <c r="A1982" s="5">
         <v>45916.39928375</v>
       </c>
@@ -53774,7 +53774,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2008" ht="22.5" customHeight="1">
+    <row r="2008" ht="22.5" hidden="1" customHeight="1">
       <c r="A2008" s="5">
         <v>45917.394830000005</v>
       </c>
@@ -54320,7 +54320,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2029" ht="22.5" customHeight="1">
+    <row r="2029" ht="22.5" hidden="1" customHeight="1">
       <c r="A2029" s="5">
         <v>45918.392201863426</v>
       </c>
@@ -54944,7 +54944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2053" ht="22.5" customHeight="1">
+    <row r="2053" ht="22.5" hidden="1" customHeight="1">
       <c r="A2053" s="5">
         <v>45919.38368543981</v>
       </c>
@@ -55412,7 +55412,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2071" ht="22.5" customHeight="1">
+    <row r="2071" ht="22.5" hidden="1" customHeight="1">
       <c r="A2071" s="5">
         <v>45922.38489828704</v>
       </c>
@@ -55828,7 +55828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2087" ht="22.5" customHeight="1">
+    <row r="2087" ht="22.5" hidden="1" customHeight="1">
       <c r="A2087" s="5">
         <v>45923.38983987269</v>
       </c>
@@ -56426,7 +56426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2110" ht="22.5" customHeight="1">
+    <row r="2110" ht="22.5" hidden="1" customHeight="1">
       <c r="A2110" s="5">
         <v>45926.40699524306</v>
       </c>
@@ -56764,7 +56764,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="2123" ht="22.5" customHeight="1">
+    <row r="2123" ht="22.5" hidden="1" customHeight="1">
       <c r="A2123" s="5">
         <v>45930.38858100695</v>
       </c>
@@ -57154,7 +57154,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2138" ht="22.5" customHeight="1">
+    <row r="2138" ht="22.5" hidden="1" customHeight="1">
       <c r="A2138" s="5">
         <v>45931.38799164352</v>
       </c>
@@ -58688,7 +58688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2197" ht="22.5" customHeight="1">
+    <row r="2197" ht="22.5" hidden="1" customHeight="1">
       <c r="A2197" s="5">
         <v>45943.45935690972</v>
       </c>
@@ -58922,7 +58922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2206" ht="22.5" customHeight="1">
+    <row r="2206" ht="22.5" hidden="1" customHeight="1">
       <c r="A2206" s="5">
         <v>45944.382605949075</v>
       </c>
@@ -59364,7 +59364,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2223" ht="22.5" customHeight="1">
+    <row r="2223" ht="22.5" hidden="1" customHeight="1">
       <c r="A2223" s="5">
         <v>45947.403554282406</v>
       </c>
@@ -59702,7 +59702,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2236" ht="22.5" customHeight="1">
+    <row r="2236" ht="22.5" hidden="1" customHeight="1">
       <c r="A2236" s="5">
         <v>45949.42311469908</v>
       </c>
@@ -60222,7 +60222,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2256" ht="22.5" customHeight="1">
+    <row r="2256" ht="22.5" hidden="1" customHeight="1">
       <c r="A2256" s="5">
         <v>45952.38742313658</v>
       </c>
@@ -60586,7 +60586,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2270" ht="22.5" customHeight="1">
+    <row r="2270" ht="22.5" hidden="1" customHeight="1">
       <c r="A2270" s="5">
         <v>45953.32561439815</v>
       </c>
@@ -61288,7 +61288,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="2297" ht="22.5" customHeight="1">
+    <row r="2297" ht="22.5" hidden="1" customHeight="1">
       <c r="A2297" s="5">
         <v>45957.37074780093</v>
       </c>
@@ -61704,7 +61704,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2313" ht="22.5" customHeight="1">
+    <row r="2313" ht="22.5" hidden="1" customHeight="1">
       <c r="A2313" s="5">
         <v>45958.35920699074</v>
       </c>
@@ -63004,7 +63004,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2363" ht="22.5" customHeight="1">
+    <row r="2363" ht="22.5" hidden="1" customHeight="1">
       <c r="A2363" s="5">
         <v>45964.400345243055</v>
       </c>
@@ -63810,7 +63810,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2394" ht="22.5" customHeight="1">
+    <row r="2394" ht="22.5" hidden="1" customHeight="1">
       <c r="A2394" s="5">
         <v>45966.37463479167</v>
       </c>
@@ -64460,7 +64460,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2419" ht="22.5" customHeight="1">
+    <row r="2419" ht="22.5" hidden="1" customHeight="1">
       <c r="A2419" s="5">
         <v>45967.390986087965</v>
       </c>
@@ -64928,7 +64928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2437" ht="22.5" customHeight="1">
+    <row r="2437" ht="22.5" hidden="1" customHeight="1">
       <c r="A2437" s="5">
         <v>45968.389227569445</v>
       </c>
@@ -65162,7 +65162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2446" ht="22.5" customHeight="1">
+    <row r="2446" ht="22.5" hidden="1" customHeight="1">
       <c r="A2446" s="5">
         <v>45979.38241262731</v>
       </c>
@@ -65552,7 +65552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2461" ht="22.5" customHeight="1">
+    <row r="2461" ht="22.5" hidden="1" customHeight="1">
       <c r="A2461" s="5">
         <v>45980.37654516204</v>
       </c>
@@ -65942,7 +65942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2476" ht="22.5" customHeight="1">
+    <row r="2476" ht="22.5" hidden="1" customHeight="1">
       <c r="A2476" s="5">
         <v>45981.38114978009</v>
       </c>
@@ -68126,7 +68126,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2560" ht="22.5" customHeight="1">
+    <row r="2560" ht="22.5" hidden="1" customHeight="1">
       <c r="A2560" s="5">
         <v>46010.6586277662</v>
       </c>
@@ -68152,7 +68152,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2561" ht="22.5" customHeight="1">
+    <row r="2561" ht="22.5" hidden="1" customHeight="1">
       <c r="A2561" s="5">
         <v>46010.6602537037</v>
       </c>
@@ -68178,7 +68178,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2562" ht="22.5" customHeight="1">
+    <row r="2562" ht="22.5" hidden="1" customHeight="1">
       <c r="A2562" s="5">
         <v>46010.68708289352</v>
       </c>
@@ -68204,7 +68204,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2563" ht="22.5" customHeight="1">
+    <row r="2563" ht="22.5" hidden="1" customHeight="1">
       <c r="A2563" s="5">
         <v>46010.68727944445</v>
       </c>
@@ -68230,7 +68230,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2564" ht="22.5" customHeight="1">
+    <row r="2564" ht="22.5" hidden="1" customHeight="1">
       <c r="A2564" s="5">
         <v>46010.68803590278</v>
       </c>
@@ -68256,7 +68256,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2565" ht="22.5" customHeight="1">
+    <row r="2565" ht="22.5" hidden="1" customHeight="1">
       <c r="A2565" s="5">
         <v>46010.68818315973</v>
       </c>
@@ -68282,7 +68282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2566" ht="22.5" customHeight="1">
+    <row r="2566" ht="22.5" hidden="1" customHeight="1">
       <c r="A2566" s="5">
         <v>46010.689745069445</v>
       </c>
@@ -68308,7 +68308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2567" ht="22.5" customHeight="1">
+    <row r="2567" ht="22.5" hidden="1" customHeight="1">
       <c r="A2567" s="5">
         <v>46010.689891331014</v>
       </c>
@@ -68334,7 +68334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2568" ht="22.5" customHeight="1">
+    <row r="2568" ht="22.5" hidden="1" customHeight="1">
       <c r="A2568" s="5">
         <v>46010.698468726856</v>
       </c>
@@ -68360,7 +68360,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2569" ht="22.5" customHeight="1">
+    <row r="2569" ht="22.5" hidden="1" customHeight="1">
       <c r="A2569" s="5">
         <v>46010.69863162037</v>
       </c>
@@ -68386,7 +68386,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2570" ht="22.5" customHeight="1">
+    <row r="2570" ht="22.5" hidden="1" customHeight="1">
       <c r="A2570" s="5">
         <v>46010.69886758101</v>
       </c>
@@ -68412,7 +68412,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2571" ht="22.5" customHeight="1">
+    <row r="2571" ht="22.5" hidden="1" customHeight="1">
       <c r="A2571" s="5">
         <v>46010.702832106486</v>
       </c>
@@ -68438,7 +68438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2572" ht="22.5" customHeight="1">
+    <row r="2572" ht="22.5" hidden="1" customHeight="1">
       <c r="A2572" s="5">
         <v>46010.70299414352</v>
       </c>
@@ -68464,7 +68464,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2573" ht="22.5" customHeight="1">
+    <row r="2573" ht="22.5" hidden="1" customHeight="1">
       <c r="A2573" s="5">
         <v>46010.70315818287</v>
       </c>
@@ -68490,7 +68490,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2574" ht="22.5" customHeight="1">
+    <row r="2574" ht="22.5" hidden="1" customHeight="1">
       <c r="A2574" s="5">
         <v>46011.36116439815</v>
       </c>
@@ -68516,7 +68516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2575" ht="22.5" customHeight="1">
+    <row r="2575" ht="22.5" hidden="1" customHeight="1">
       <c r="A2575" s="5">
         <v>46011.36194297454</v>
       </c>
@@ -68542,7 +68542,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2576" ht="22.5" customHeight="1">
+    <row r="2576" ht="22.5" hidden="1" customHeight="1">
       <c r="A2576" s="5">
         <v>46011.36257939815</v>
       </c>
@@ -68568,7 +68568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2577" ht="22.5" customHeight="1">
+    <row r="2577" ht="22.5" hidden="1" customHeight="1">
       <c r="A2577" s="5">
         <v>46011.36303930556</v>
       </c>
@@ -68594,7 +68594,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2578" ht="22.5" customHeight="1">
+    <row r="2578" ht="22.5" hidden="1" customHeight="1">
       <c r="A2578" s="5">
         <v>46011.36370047454</v>
       </c>
@@ -68620,7 +68620,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="2579" ht="22.5" customHeight="1">
+    <row r="2579" ht="22.5" hidden="1" customHeight="1">
       <c r="A2579" s="5">
         <v>46011.364157986114</v>
       </c>
@@ -68646,7 +68646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2580" ht="22.5" customHeight="1">
+    <row r="2580" ht="22.5" hidden="1" customHeight="1">
       <c r="A2580" s="5">
         <v>46011.36491052083</v>
       </c>
@@ -68672,7 +68672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2581" ht="22.5" customHeight="1">
+    <row r="2581" ht="22.5" hidden="1" customHeight="1">
       <c r="A2581" s="5">
         <v>46011.36641270833</v>
       </c>
@@ -68698,7 +68698,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2582" ht="22.5" customHeight="1">
+    <row r="2582" ht="22.5" hidden="1" customHeight="1">
       <c r="A2582" s="5">
         <v>46011.36754990741</v>
       </c>
@@ -68724,7 +68724,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2583" ht="22.5" customHeight="1">
+    <row r="2583" ht="22.5" hidden="1" customHeight="1">
       <c r="A2583" s="5">
         <v>46011.3680284375</v>
       </c>
@@ -68750,7 +68750,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2584" ht="22.5" customHeight="1">
+    <row r="2584" ht="22.5" hidden="1" customHeight="1">
       <c r="A2584" s="5">
         <v>46011.36899107639</v>
       </c>
@@ -68776,7 +68776,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2585" ht="22.5" customHeight="1">
+    <row r="2585" ht="22.5" hidden="1" customHeight="1">
       <c r="A2585" s="5">
         <v>46011.36956982639</v>
       </c>
@@ -68802,7 +68802,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2586" ht="22.5" customHeight="1">
+    <row r="2586" ht="22.5" hidden="1" customHeight="1">
       <c r="A2586" s="5">
         <v>46011.36990143519</v>
       </c>
@@ -68828,7 +68828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2587" ht="22.5" customHeight="1">
+    <row r="2587" ht="22.5" hidden="1" customHeight="1">
       <c r="A2587" s="5">
         <v>46011.37083474537</v>
       </c>
@@ -68854,7 +68854,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2588" ht="22.5" customHeight="1">
+    <row r="2588" ht="22.5" hidden="1" customHeight="1">
       <c r="A2588" s="5">
         <v>46011.37155277778</v>
       </c>
@@ -68880,7 +68880,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="2589" ht="22.5" customHeight="1">
+    <row r="2589" ht="22.5" hidden="1" customHeight="1">
       <c r="A2589" s="5">
         <v>46011.37188224537</v>
       </c>
@@ -68906,7 +68906,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2590" ht="22.5" customHeight="1">
+    <row r="2590" ht="22.5" hidden="1" customHeight="1">
       <c r="A2590" s="5">
         <v>46011.37250920139</v>
       </c>
@@ -68932,7 +68932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2591" ht="22.5" customHeight="1">
+    <row r="2591" ht="22.5" hidden="1" customHeight="1">
       <c r="A2591" s="5">
         <v>46011.37290135417</v>
       </c>
@@ -68958,7 +68958,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2592" ht="22.5" customHeight="1">
+    <row r="2592" ht="22.5" hidden="1" customHeight="1">
       <c r="A2592" s="5">
         <v>46011.644947673616</v>
       </c>
@@ -68984,7 +68984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2593" ht="22.5" customHeight="1">
+    <row r="2593" ht="22.5" hidden="1" customHeight="1">
       <c r="A2593" s="5">
         <v>46011.64575946759</v>
       </c>
@@ -69010,7 +69010,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2594" ht="22.5" customHeight="1">
+    <row r="2594" ht="22.5" hidden="1" customHeight="1">
       <c r="A2594" s="5">
         <v>46011.64679453704</v>
       </c>
@@ -69036,7 +69036,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2595" ht="22.5" customHeight="1">
+    <row r="2595" ht="22.5" hidden="1" customHeight="1">
       <c r="A2595" s="5">
         <v>46011.64726376157</v>
       </c>
@@ -69062,7 +69062,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2596" ht="22.5" customHeight="1">
+    <row r="2596" ht="22.5" hidden="1" customHeight="1">
       <c r="A2596" s="5">
         <v>46011.64855503472</v>
       </c>
@@ -69088,7 +69088,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2597" ht="22.5" customHeight="1">
+    <row r="2597" ht="22.5" hidden="1" customHeight="1">
       <c r="A2597" s="5">
         <v>46011.65217178241</v>
       </c>
@@ -69114,7 +69114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2598" ht="22.5" customHeight="1">
+    <row r="2598" ht="22.5" hidden="1" customHeight="1">
       <c r="A2598" s="5">
         <v>46011.65270490741</v>
       </c>
@@ -69140,7 +69140,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2599" ht="22.5" customHeight="1">
+    <row r="2599" ht="22.5" hidden="1" customHeight="1">
       <c r="A2599" s="5">
         <v>46011.65336935185</v>
       </c>
@@ -69166,7 +69166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2600" ht="22.5" customHeight="1">
+    <row r="2600" ht="22.5" hidden="1" customHeight="1">
       <c r="A2600" s="5">
         <v>46011.65512840278</v>
       </c>
@@ -69192,7 +69192,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2601" ht="22.5" customHeight="1">
+    <row r="2601" ht="22.5" hidden="1" customHeight="1">
       <c r="A2601" s="5">
         <v>46011.655611504626</v>
       </c>
@@ -69218,7 +69218,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2602" ht="22.5" customHeight="1">
+    <row r="2602" ht="22.5" hidden="1" customHeight="1">
       <c r="A2602" s="5">
         <v>46011.65925834491</v>
       </c>
@@ -69244,7 +69244,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2603" ht="22.5" customHeight="1">
+    <row r="2603" ht="22.5" hidden="1" customHeight="1">
       <c r="A2603" s="5">
         <v>46011.65957847222</v>
       </c>
@@ -69270,7 +69270,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2604" ht="22.5" customHeight="1">
+    <row r="2604" ht="22.5" hidden="1" customHeight="1">
       <c r="A2604" s="5">
         <v>46011.659953912036</v>
       </c>
@@ -69296,7 +69296,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2605" ht="22.5" customHeight="1">
+    <row r="2605" ht="22.5" hidden="1" customHeight="1">
       <c r="A2605" s="5">
         <v>46011.66039179398</v>
       </c>
@@ -69322,7 +69322,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2606" ht="22.5" customHeight="1">
+    <row r="2606" ht="22.5" hidden="1" customHeight="1">
       <c r="A2606" s="5">
         <v>46011.66075746527</v>
       </c>
@@ -69348,7 +69348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2607" ht="22.5" customHeight="1">
+    <row r="2607" ht="22.5" hidden="1" customHeight="1">
       <c r="A2607" s="5">
         <v>46011.661354814816</v>
       </c>
@@ -69374,7 +69374,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2608" ht="22.5" customHeight="1">
+    <row r="2608" ht="22.5" hidden="1" customHeight="1">
       <c r="A2608" s="5">
         <v>46011.66189505787</v>
       </c>
@@ -69400,7 +69400,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2609" ht="22.5" customHeight="1">
+    <row r="2609" ht="22.5" hidden="1" customHeight="1">
       <c r="A2609" s="5">
         <v>46011.66219752315</v>
       </c>
@@ -69426,7 +69426,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2610" ht="22.5" customHeight="1">
+    <row r="2610" ht="22.5" hidden="1" customHeight="1">
       <c r="A2610" s="5">
         <v>46011.662445787035</v>
       </c>
@@ -69452,7 +69452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2611" ht="22.5" customHeight="1">
+    <row r="2611" ht="22.5" hidden="1" customHeight="1">
       <c r="A2611" s="5">
         <v>46011.662733310186</v>
       </c>
@@ -69478,7 +69478,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2612" ht="22.5" customHeight="1">
+    <row r="2612" ht="22.5" hidden="1" customHeight="1">
       <c r="A2612" s="5">
         <v>46011.66310677084</v>
       </c>
@@ -69504,7 +69504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2613" ht="22.5" customHeight="1">
+    <row r="2613" ht="22.5" hidden="1" customHeight="1">
       <c r="A2613" s="5">
         <v>46011.663499953705</v>
       </c>
@@ -69530,7 +69530,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2614" ht="22.5" customHeight="1">
+    <row r="2614" ht="22.5" hidden="1" customHeight="1">
       <c r="A2614" s="5">
         <v>46011.66377085648</v>
       </c>
@@ -69556,7 +69556,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2615" ht="22.5" customHeight="1">
+    <row r="2615" ht="22.5" hidden="1" customHeight="1">
       <c r="A2615" s="5">
         <v>46011.664039166666</v>
       </c>
@@ -69582,7 +69582,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2616" ht="22.5" customHeight="1">
+    <row r="2616" ht="22.5" hidden="1" customHeight="1">
       <c r="A2616" s="5">
         <v>46011.66431335648</v>
       </c>
@@ -69608,7 +69608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2617" ht="22.5" customHeight="1">
+    <row r="2617" ht="22.5" hidden="1" customHeight="1">
       <c r="A2617" s="5">
         <v>46012.406275416666</v>
       </c>
@@ -69634,7 +69634,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2618" ht="22.5" customHeight="1">
+    <row r="2618" ht="22.5" hidden="1" customHeight="1">
       <c r="A2618" s="5">
         <v>46012.40696774305</v>
       </c>
@@ -69660,7 +69660,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2619" ht="22.5" customHeight="1">
+    <row r="2619" ht="22.5" hidden="1" customHeight="1">
       <c r="A2619" s="5">
         <v>46012.40735553241</v>
       </c>
@@ -69686,7 +69686,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2620" ht="22.5" customHeight="1">
+    <row r="2620" ht="22.5" hidden="1" customHeight="1">
       <c r="A2620" s="5">
         <v>46012.407736747686</v>
       </c>
@@ -69712,7 +69712,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2621" ht="22.5" customHeight="1">
+    <row r="2621" ht="22.5" hidden="1" customHeight="1">
       <c r="A2621" s="5">
         <v>46012.40803497685</v>
       </c>
@@ -69738,7 +69738,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2622" ht="22.5" customHeight="1">
+    <row r="2622" ht="22.5" hidden="1" customHeight="1">
       <c r="A2622" s="5">
         <v>46012.408312280095</v>
       </c>
@@ -69764,7 +69764,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2623" ht="22.5" customHeight="1">
+    <row r="2623" ht="22.5" hidden="1" customHeight="1">
       <c r="A2623" s="5">
         <v>46012.408646076394</v>
       </c>
@@ -69790,7 +69790,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2624" ht="22.5" customHeight="1">
+    <row r="2624" ht="22.5" hidden="1" customHeight="1">
       <c r="A2624" s="5">
         <v>46012.409001064814</v>
       </c>
@@ -69816,7 +69816,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2625" ht="22.5" customHeight="1">
+    <row r="2625" ht="22.5" hidden="1" customHeight="1">
       <c r="A2625" s="5">
         <v>46012.409509398145</v>
       </c>
@@ -69842,7 +69842,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2626" ht="22.5" customHeight="1">
+    <row r="2626" ht="22.5" hidden="1" customHeight="1">
       <c r="A2626" s="5">
         <v>46012.409934525465</v>
       </c>
@@ -69868,7 +69868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2627" ht="22.5" customHeight="1">
+    <row r="2627" ht="22.5" hidden="1" customHeight="1">
       <c r="A2627" s="5">
         <v>46012.410468587965</v>
       </c>
@@ -69894,7 +69894,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2628" ht="22.5" customHeight="1">
+    <row r="2628" ht="22.5" hidden="1" customHeight="1">
       <c r="A2628" s="5">
         <v>46012.41076921296</v>
       </c>
@@ -69920,7 +69920,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2629" ht="22.5" customHeight="1">
+    <row r="2629" ht="22.5" hidden="1" customHeight="1">
       <c r="A2629" s="5">
         <v>46012.41105765046</v>
       </c>
@@ -69946,7 +69946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2630" ht="22.5" customHeight="1">
+    <row r="2630" ht="22.5" hidden="1" customHeight="1">
       <c r="A2630" s="5">
         <v>46012.411354027776</v>
       </c>
@@ -69972,7 +69972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2631" ht="22.5" customHeight="1">
+    <row r="2631" ht="22.5" hidden="1" customHeight="1">
       <c r="A2631" s="5">
         <v>46012.411611435185</v>
       </c>
@@ -69998,7 +69998,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2632" ht="22.5" customHeight="1">
+    <row r="2632" ht="22.5" hidden="1" customHeight="1">
       <c r="A2632" s="5">
         <v>46012.41193630787</v>
       </c>
@@ -70024,7 +70024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2633" ht="22.5" customHeight="1">
+    <row r="2633" ht="22.5" hidden="1" customHeight="1">
       <c r="A2633" s="5">
         <v>46012.41230246528</v>
       </c>
@@ -70050,7 +70050,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2634" ht="22.5" customHeight="1">
+    <row r="2634" ht="22.5" hidden="1" customHeight="1">
       <c r="A2634" s="5">
         <v>46012.416488877316</v>
       </c>
@@ -70076,7 +70076,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2635" ht="22.5" customHeight="1">
+    <row r="2635" ht="22.5" hidden="1" customHeight="1">
       <c r="A2635" s="5">
         <v>46012.41720302083</v>
       </c>
@@ -70102,7 +70102,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2636" ht="22.5" customHeight="1">
+    <row r="2636" ht="22.5" hidden="1" customHeight="1">
       <c r="A2636" s="5">
         <v>46012.417760729164</v>
       </c>
@@ -70128,7 +70128,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2637" ht="22.5" customHeight="1">
+    <row r="2637" ht="22.5" hidden="1" customHeight="1">
       <c r="A2637" s="5">
         <v>46012.417966493056</v>
       </c>
@@ -70154,7 +70154,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2638" ht="22.5" customHeight="1">
+    <row r="2638" ht="22.5" hidden="1" customHeight="1">
       <c r="A2638" s="5">
         <v>46013.335654027775</v>
       </c>
@@ -70180,7 +70180,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2639" ht="22.5" customHeight="1">
+    <row r="2639" ht="22.5" hidden="1" customHeight="1">
       <c r="A2639" s="5">
         <v>46013.33618799769</v>
       </c>
@@ -70206,7 +70206,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2640" ht="22.5" customHeight="1">
+    <row r="2640" ht="22.5" hidden="1" customHeight="1">
       <c r="A2640" s="5">
         <v>46013.33657557871</v>
       </c>
@@ -70232,7 +70232,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2641" ht="22.5" customHeight="1">
+    <row r="2641" ht="22.5" hidden="1" customHeight="1">
       <c r="A2641" s="5">
         <v>46013.33698266203</v>
       </c>
@@ -70258,7 +70258,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2642" ht="22.5" customHeight="1">
+    <row r="2642" ht="22.5" hidden="1" customHeight="1">
       <c r="A2642" s="5">
         <v>46013.33732827546</v>
       </c>
@@ -70284,7 +70284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2643" ht="22.5" customHeight="1">
+    <row r="2643" ht="22.5" hidden="1" customHeight="1">
       <c r="A2643" s="5">
         <v>46013.33771087963</v>
       </c>
@@ -70310,7 +70310,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2644" ht="22.5" customHeight="1">
+    <row r="2644" ht="22.5" hidden="1" customHeight="1">
       <c r="A2644" s="5">
         <v>46013.33834283565</v>
       </c>
@@ -70336,7 +70336,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2645" ht="22.5" customHeight="1">
+    <row r="2645" ht="22.5" hidden="1" customHeight="1">
       <c r="A2645" s="5">
         <v>46013.34011751157</v>
       </c>
@@ -70362,7 +70362,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2646" ht="22.5" customHeight="1">
+    <row r="2646" ht="22.5" hidden="1" customHeight="1">
       <c r="A2646" s="5">
         <v>46013.342919675924</v>
       </c>
@@ -70388,7 +70388,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2647" ht="22.5" customHeight="1">
+    <row r="2647" ht="22.5" hidden="1" customHeight="1">
       <c r="A2647" s="5">
         <v>46013.343977303244</v>
       </c>
@@ -70414,7 +70414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2648" ht="22.5" customHeight="1">
+    <row r="2648" ht="22.5" hidden="1" customHeight="1">
       <c r="A2648" s="5">
         <v>46013.35667259259</v>
       </c>
@@ -70440,7 +70440,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2649" ht="22.5" customHeight="1">
+    <row r="2649" ht="22.5" hidden="1" customHeight="1">
       <c r="A2649" s="5">
         <v>46013.3570225</v>
       </c>
@@ -70466,7 +70466,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2650" ht="22.5" customHeight="1">
+    <row r="2650" ht="22.5" hidden="1" customHeight="1">
       <c r="A2650" s="5">
         <v>46013.357438391206</v>
       </c>
@@ -70492,7 +70492,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2651" ht="22.5" customHeight="1">
+    <row r="2651" ht="22.5" hidden="1" customHeight="1">
       <c r="A2651" s="5">
         <v>46013.35799391204</v>
       </c>
@@ -70518,7 +70518,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2652" ht="22.5" customHeight="1">
+    <row r="2652" ht="22.5" hidden="1" customHeight="1">
       <c r="A2652" s="5">
         <v>46013.3583334838</v>
       </c>
@@ -70544,7 +70544,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2653" ht="22.5" customHeight="1">
+    <row r="2653" ht="22.5" hidden="1" customHeight="1">
       <c r="A2653" s="5">
         <v>46013.358621203704</v>
       </c>
@@ -70570,7 +70570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2654" ht="22.5" customHeight="1">
+    <row r="2654" ht="22.5" hidden="1" customHeight="1">
       <c r="A2654" s="5">
         <v>46013.35895483797</v>
       </c>
@@ -70596,7 +70596,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2655" ht="22.5" customHeight="1">
+    <row r="2655" ht="22.5" hidden="1" customHeight="1">
       <c r="A2655" s="5">
         <v>46013.35930568287</v>
       </c>
@@ -70622,7 +70622,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2656" ht="22.5" customHeight="1">
+    <row r="2656" ht="22.5" hidden="1" customHeight="1">
       <c r="A2656" s="5">
         <v>46013.36087318287</v>
       </c>
@@ -70648,7 +70648,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2657" ht="22.5" customHeight="1">
+    <row r="2657" ht="22.5" hidden="1" customHeight="1">
       <c r="A2657" s="5">
         <v>46013.36119708333</v>
       </c>
@@ -70674,7 +70674,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2658" ht="22.5" customHeight="1">
+    <row r="2658" ht="22.5" hidden="1" customHeight="1">
       <c r="A2658" s="5">
         <v>46013.362917997685</v>
       </c>
@@ -70700,7 +70700,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="2659" ht="22.5" customHeight="1">
+    <row r="2659" ht="22.5" hidden="1" customHeight="1">
       <c r="A2659" s="5">
         <v>46013.36359679398</v>
       </c>
@@ -70726,7 +70726,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2660" ht="22.5" customHeight="1">
+    <row r="2660" ht="22.5" hidden="1" customHeight="1">
       <c r="A2660" s="5">
         <v>46013.364556238426</v>
       </c>
@@ -70752,7 +70752,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2661" ht="22.5" customHeight="1">
+    <row r="2661" ht="22.5" hidden="1" customHeight="1">
       <c r="A2661" s="5">
         <v>46013.375676701384</v>
       </c>
@@ -70778,7 +70778,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2662" ht="22.5" customHeight="1">
+    <row r="2662" ht="22.5" hidden="1" customHeight="1">
       <c r="A2662" s="5">
         <v>46013.376511400464</v>
       </c>
@@ -70804,13 +70804,1235 @@
         <v>13</v>
       </c>
     </row>
+    <row r="2663" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2663" s="5">
+        <v>46013.63638091435</v>
+      </c>
+      <c r="B2663" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2663" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2663" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2663" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2663" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2663" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2663" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2664" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2664" s="5">
+        <v>46013.64290060185</v>
+      </c>
+      <c r="B2664" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2664" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2664" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2664" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2664" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2664" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2664" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2665" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2665" s="5">
+        <v>46013.644082893516</v>
+      </c>
+      <c r="B2665" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2665" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2665" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2665" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2665" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2665" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2665" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2666" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2666" s="5">
+        <v>46013.646062245374</v>
+      </c>
+      <c r="B2666" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2666" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2666" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2666" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2666" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2666" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2666" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2667" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2667" s="5">
+        <v>46013.64692101852</v>
+      </c>
+      <c r="B2667" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2667" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2667" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2667" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2667" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2667" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2667" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2668" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2668" s="5">
+        <v>46013.65180277778</v>
+      </c>
+      <c r="B2668" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2668" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2668" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2668" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2668" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2668" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2668" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2669" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2669" s="5">
+        <v>46013.65762892361</v>
+      </c>
+      <c r="B2669" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2669" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2669" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2669" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2669" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2669" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2669" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2670" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2670" s="5">
+        <v>46013.6579621875</v>
+      </c>
+      <c r="B2670" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2670" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2670" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2670" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2670" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2670" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2670" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2671" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2671" s="5">
+        <v>46013.66350510417</v>
+      </c>
+      <c r="B2671" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2671" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2671" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2671" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2671" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2671" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2671" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2672" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2672" s="5">
+        <v>46013.663840381945</v>
+      </c>
+      <c r="B2672" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2672" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2672" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2672" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2672" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2672" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2672" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2673" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2673" s="5">
+        <v>46013.66417862268</v>
+      </c>
+      <c r="B2673" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2673" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2673" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2673" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2673" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2673" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2673" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2674" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2674" s="5">
+        <v>46013.664499108796</v>
+      </c>
+      <c r="B2674" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2674" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2674" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2674" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2674" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2674" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2674" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2675" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2675" s="5">
+        <v>46013.6647893287</v>
+      </c>
+      <c r="B2675" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2675" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2675" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2675" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2675" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2675" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2675" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2676" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2676" s="5">
+        <v>46013.665156006944</v>
+      </c>
+      <c r="B2676" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2676" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D2676" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2676" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2676" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2676" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2676" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2677" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2677" s="5">
+        <v>46013.66688496528</v>
+      </c>
+      <c r="B2677" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2677" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2677" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2677" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2677" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2677" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2677" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2678" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2678" s="5">
+        <v>46013.66868671296</v>
+      </c>
+      <c r="B2678" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2678" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2678" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2678" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2678" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2678" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2678" s="6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="2679" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2679" s="5">
+        <v>46013.670060358796</v>
+      </c>
+      <c r="B2679" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2679" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2679" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2679" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2679" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2679" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2679" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2680" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2680" s="5">
+        <v>46013.67331460648</v>
+      </c>
+      <c r="B2680" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2680" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2680" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2680" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2680" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2680" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2680" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2681" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2681" s="5">
+        <v>46013.6736204051</v>
+      </c>
+      <c r="B2681" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2681" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2681" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2681" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2681" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2681" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2681" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2682" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2682" s="5">
+        <v>46013.67488200231</v>
+      </c>
+      <c r="B2682" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2682" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2682" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2682" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2682" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2682" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2682" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2683" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2683" s="5">
+        <v>46013.68261574074</v>
+      </c>
+      <c r="B2683" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2683" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2683" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2683" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2683" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2683" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2683" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2684" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2684" s="5">
+        <v>46013.68291307871</v>
+      </c>
+      <c r="B2684" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2684" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2684" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2684" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2684" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2684" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2684" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2685" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2685" s="5">
+        <v>46013.68362329861</v>
+      </c>
+      <c r="B2685" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2685" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2685" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2685" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2685" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2685" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2685" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2686" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2686" s="5">
+        <v>46013.68426207176</v>
+      </c>
+      <c r="B2686" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2686" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2686" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2686" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2686" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2686" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2686" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2687" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2687" s="5">
+        <v>46013.68832883102</v>
+      </c>
+      <c r="B2687" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2687" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D2687" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2687" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2687" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2687" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2687" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2688" ht="22.5" hidden="1" customHeight="1">
+      <c r="A2688" s="5">
+        <v>46013.688577152774</v>
+      </c>
+      <c r="B2688" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2688" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2688" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2688" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2688" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2688" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2688" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2689" ht="22.5" customHeight="1">
+      <c r="A2689" s="5">
+        <v>46014.355254062495</v>
+      </c>
+      <c r="B2689" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2689" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="D2689" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2689" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2689" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2689" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2689" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2690" ht="22.5" customHeight="1">
+      <c r="A2690" s="5">
+        <v>46014.366081238426</v>
+      </c>
+      <c r="B2690" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2690" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D2690" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2690" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2690" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2690" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2690" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2691" ht="22.5" customHeight="1">
+      <c r="A2691" s="5">
+        <v>46014.366509178246</v>
+      </c>
+      <c r="B2691" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2691" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2691" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2691" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2691" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2691" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2691" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2692" ht="22.5" customHeight="1">
+      <c r="A2692" s="5">
+        <v>46014.36729189815</v>
+      </c>
+      <c r="B2692" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2692" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2692" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2692" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2692" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2692" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2692" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2693" ht="22.5" customHeight="1">
+      <c r="A2693" s="5">
+        <v>46014.36779369213</v>
+      </c>
+      <c r="B2693" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2693" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D2693" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2693" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2693" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2693" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2693" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2694" ht="22.5" customHeight="1">
+      <c r="A2694" s="5">
+        <v>46014.368286620374</v>
+      </c>
+      <c r="B2694" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2694" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2694" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2694" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2694" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2694" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2694" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2695" ht="22.5" customHeight="1">
+      <c r="A2695" s="5">
+        <v>46014.36884717592</v>
+      </c>
+      <c r="B2695" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2695" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2695" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2695" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2695" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2695" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2695" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2696" ht="22.5" customHeight="1">
+      <c r="A2696" s="5">
+        <v>46014.369300185186</v>
+      </c>
+      <c r="B2696" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2696" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2696" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2696" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2696" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2696" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2696" s="6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2697" ht="22.5" customHeight="1">
+      <c r="A2697" s="5">
+        <v>46014.36972478009</v>
+      </c>
+      <c r="B2697" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2697" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2697" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2697" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2697" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2697" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2697" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2698" ht="22.5" customHeight="1">
+      <c r="A2698" s="5">
+        <v>46014.37022012731</v>
+      </c>
+      <c r="B2698" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2698" s="6" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2698" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2698" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2698" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2698" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2698" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2699" ht="22.5" customHeight="1">
+      <c r="A2699" s="5">
+        <v>46014.37053568287</v>
+      </c>
+      <c r="B2699" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2699" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2699" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2699" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2699" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2699" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2699" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2700" ht="22.5" customHeight="1">
+      <c r="A2700" s="5">
+        <v>46014.37097525463</v>
+      </c>
+      <c r="B2700" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2700" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2700" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2700" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2700" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2700" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2700" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2701" ht="22.5" customHeight="1">
+      <c r="A2701" s="5">
+        <v>46014.37143585648</v>
+      </c>
+      <c r="B2701" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2701" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="D2701" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2701" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2701" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2701" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2701" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2702" ht="22.5" customHeight="1">
+      <c r="A2702" s="5">
+        <v>46014.37370295139</v>
+      </c>
+      <c r="B2702" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2702" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2702" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2702" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2702" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2702" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2702" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="2703" ht="22.5" customHeight="1">
+      <c r="A2703" s="5">
+        <v>46014.374090625</v>
+      </c>
+      <c r="B2703" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2703" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D2703" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2703" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2703" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2703" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2703" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2704" ht="22.5" customHeight="1">
+      <c r="A2704" s="5">
+        <v>46014.374461886575</v>
+      </c>
+      <c r="B2704" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2704" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2704" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2704" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2704" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2704" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2704" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2705" ht="22.5" customHeight="1">
+      <c r="A2705" s="5">
+        <v>46014.374851342596</v>
+      </c>
+      <c r="B2705" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2705" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2705" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2705" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2705" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2705" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2705" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2706" ht="22.5" customHeight="1">
+      <c r="A2706" s="5">
+        <v>46014.375244062496</v>
+      </c>
+      <c r="B2706" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2706" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2706" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2706" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2706" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2706" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2706" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2707" ht="22.5" customHeight="1">
+      <c r="A2707" s="5">
+        <v>46014.37572994213</v>
+      </c>
+      <c r="B2707" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2707" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2707" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2707" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2707" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2707" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2707" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2708" ht="22.5" customHeight="1">
+      <c r="A2708" s="5">
+        <v>46014.37598351852</v>
+      </c>
+      <c r="B2708" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2708" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="D2708" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2708" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2708" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2708" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2708" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2709" ht="22.5" customHeight="1">
+      <c r="A2709" s="5">
+        <v>46014.377127314816</v>
+      </c>
+      <c r="B2709" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C2709" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2709" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2709" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2709" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2709" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2709" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D2762">
+  <conditionalFormatting sqref="D1:D2809">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="&quot;Muy cansado&quot;">
       <formula>NOT(ISERROR(SEARCH(("""Muy cansado"""),(D1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G2762">
+  <conditionalFormatting sqref="G2:G2809">
     <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="adolorido">
       <formula>NOT(ISERROR(SEARCH(("adolorido"),(G2))))</formula>
     </cfRule>

</xml_diff>